<commit_message>
get data from other sheet and display them as cards in the home page, change line chart to mixed chart to improve the data visualisation, intergrate the style sheet by using MDBoostrap
</commit_message>
<xml_diff>
--- a/prince.xlsx
+++ b/prince.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C653B21D-4C1F-4D5D-A25F-2F2F30015F79}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="albums" sheetId="2" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="238">
   <si>
     <t>https://www.complex.com/style/2018/06/visual-history-of-princes-album-covers/</t>
   </si>
@@ -38,9 +37,6 @@
     <t>Album</t>
   </si>
   <si>
-    <t>Peak chart positions</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
@@ -174,9 +170,6 @@
   </si>
   <si>
     <t>Crystal Ball / The Truth</t>
-  </si>
-  <si>
-    <t>Lotusflow3r / MPLSound (released as a 3-CD set together withElixer by Bria Valente)</t>
   </si>
   <si>
     <t>Plectrumelectrum [C]</t>
@@ -1962,9 +1955,6 @@
     <t>http://princevault.com/index.php?title=Album:_One_Nite_Alone..._The_Aftershow:_It_Ain%27t_Over</t>
   </si>
   <si>
-    <t>One Nite Alone… The Aftershow: It Ain't Over</t>
-  </si>
-  <si>
     <r>
       <t>One Nite Alone... The Aftershow: It Ain't Over</t>
     </r>
@@ -3631,12 +3621,6 @@
     <t>album covers and text</t>
   </si>
   <si>
-    <t>total weeks in US Charts</t>
-  </si>
-  <si>
-    <t>Album about URL</t>
-  </si>
-  <si>
     <t>weeks_in_top_100charts</t>
   </si>
   <si>
@@ -3649,14 +3633,185 @@
     <t>worldwide_Sales</t>
   </si>
   <si>
-    <t xml:space="preserve"> (June 2018) (http://prince.org/msg/7/450866)</t>
+    <t>Album_about_URL</t>
+  </si>
+  <si>
+    <t>total_weeks_in_US_Charts</t>
+  </si>
+  <si>
+    <t>Lotusflow3r</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/7/7a/For_you.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/e/ea/Prince.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/3/30/Dirtymind.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/d/dc/Controversy.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/4/49/1999-1LP.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/1/1c/Purplerain.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/2/28/Atwiad.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/8/89/Parade.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/a/aa/Sott.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/e/ee/Lovesexy.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/0/09/Batman.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/c/c1/Graffitibridge.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/f/fd/Diamondsandpearls.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/c/c8/Symbolalbum.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/a/a4/Thehits1.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/9/9f/Thehits2.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/b/b3/Thehitsthebsides.jpg/200px-Thehitsthebsides.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/4/4c/Come.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/1/1d/Blackalbum.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/1/1b/Thegoldexperience.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/0/02/Chaosanddisorder.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/0/0e/Emancipation.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/e/eb/Crystalball_album.png</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/8/81/Thetruth_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/e/e2/Thevault...oldfriends4sale_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/7/74/Raveun2thejoyfantastic_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/4/45/Ravein2thejoyfantastic_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/7/74/Theverybestof_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/c/c3/Rainbowchildren_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/f/fc/Onenitealone..._album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/c/c9/Onenitealone...live%21_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/7/73/Itaintover_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/9/99/Xpectation_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/0/08/News_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/f/f1/Musicology_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/c/cf/Chocolateinvasion_album.png</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/9/98/Slaughterhouse_album.png</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/5/5d/C-Note_album.png</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/b/b8/3121_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/a/a7/Ultimate_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/9/99/Planetearth_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/5/5d/Indigonights.png</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/2/28/Lotusflow3r_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/4/43/Mplsound_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/f/f9/20Ten_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/5/56/Plectrumelectrum_album.jpg/200px-Plectrumelectrum_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/f/fc/Artofficialage_album.jpg/200px-Artofficialage_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/c/c9/Hitnrun_album.jpg/200px-Hitnrun_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/4/47/Hitnrun_PHASEII_album.jpg/200px-Hitnrun_PHASEII_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/0/09/Prince4ever_album.jpg/200px-Prince4ever_album.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/1/1f/Purplerain_Deluxe.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/d/df/Anthology1995-2010.jpg/200px-Anthology1995-2010.jpg</t>
+  </si>
+  <si>
+    <t>http://princevault.com/images/thumb/8/80/Piano%26amicrophone1983.jpg/200px-Piano%26amicrophone1983.jpg</t>
+  </si>
+  <si>
+    <t>The Aftershow: It Ain't Over</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3739,6 +3894,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3763,10 +3926,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3777,8 +3941,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4056,2288 +4222,2448 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="39.5546875" customWidth="1"/>
-    <col min="4" max="4" width="58" customWidth="1"/>
-    <col min="5" max="5" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="58" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="16" width="8.88671875" customWidth="1"/>
+    <col min="17" max="17" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
+        <v>181</v>
+      </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E2" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1978</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2">
+        <v>200000</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>156</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1979</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3">
+        <v>2000000</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3">
+        <v>92</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1978</v>
+        <v>1980</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="E4">
+        <v>1000000</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G4">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>79</v>
       </c>
       <c r="Q4">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1979</v>
+        <v>1981</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>2000000</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G5">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
       </c>
       <c r="M5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5">
-        <v>92</v>
+        <v>15</v>
+      </c>
+      <c r="P5" t="s">
+        <v>15</v>
       </c>
       <c r="Q5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="R5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1980</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>1982</v>
+      </c>
+      <c r="B6">
+        <v>1999</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
       </c>
       <c r="E6">
-        <v>1000000</v>
+        <v>6000000</v>
       </c>
       <c r="F6">
+        <v>121</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6">
         <v>23</v>
       </c>
-      <c r="G6">
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6">
         <v>45</v>
       </c>
-      <c r="H6" t="s">
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6">
+        <v>51</v>
+      </c>
+      <c r="Q6">
+        <v>28</v>
+      </c>
+      <c r="R6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1984</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7">
+        <v>21000000</v>
+      </c>
+      <c r="F7">
+        <v>124</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1985</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>4000000</v>
+      </c>
+      <c r="F8">
+        <v>44</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
         <v>16</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
         <v>16</v>
       </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6">
-        <v>79</v>
-      </c>
-      <c r="Q6">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1981</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7">
-        <v>2000000</v>
-      </c>
-      <c r="F7">
-        <v>34</v>
-      </c>
-      <c r="G7">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>55</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7">
-        <v>50</v>
-      </c>
-      <c r="M7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1982</v>
-      </c>
-      <c r="B8">
-        <v>1999</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8">
-        <v>6000000</v>
-      </c>
-      <c r="F8">
-        <v>121</v>
-      </c>
-      <c r="G8">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1986</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <v>4000000</v>
+      </c>
+      <c r="F9">
+        <v>29</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
         <v>7</v>
       </c>
-      <c r="H8">
-        <v>35</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8">
-        <v>23</v>
-      </c>
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8">
-        <v>45</v>
-      </c>
-      <c r="M8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8">
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9">
         <v>6</v>
-      </c>
-      <c r="O8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8">
-        <v>51</v>
-      </c>
-      <c r="Q8">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1984</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9">
-        <v>21000000</v>
-      </c>
-      <c r="F9">
-        <v>124</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>5</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
         <v>2</v>
-      </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="P9">
-        <v>7</v>
       </c>
       <c r="Q9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1985</v>
+        <v>1987</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10">
         <v>4000000</v>
       </c>
       <c r="F10">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>27</v>
+      </c>
+      <c r="K10">
+        <v>11</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
         <v>1</v>
       </c>
-      <c r="H10">
-        <v>12</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>16</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
-      </c>
-      <c r="N10">
-        <v>16</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>8</v>
-      </c>
       <c r="Q10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="R10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1986</v>
+        <v>1988</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E11">
-        <v>4000000</v>
+        <v>2000000</v>
       </c>
       <c r="F11">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>8</v>
       </c>
       <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
         <v>7</v>
       </c>
-      <c r="J11">
-        <v>11</v>
-      </c>
       <c r="K11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>1987</v>
+        <v>1989</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E12">
         <v>4000000</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>2</v>
       </c>
-      <c r="J12">
-        <v>27</v>
-      </c>
-      <c r="K12">
-        <v>11</v>
-      </c>
-      <c r="L12">
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
         <v>2</v>
-      </c>
-      <c r="M12">
-        <v>3</v>
-      </c>
-      <c r="N12">
-        <v>6</v>
-      </c>
-      <c r="O12">
-        <v>6</v>
       </c>
       <c r="P12">
         <v>1</v>
       </c>
       <c r="Q12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1988</v>
+        <v>1990</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E13">
         <v>2000000</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
         <v>8</v>
       </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
       <c r="J13">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="K13">
         <v>4</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M13">
         <v>2</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1989</v>
+        <v>1991</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>45</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E14">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="F14">
+        <v>46</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
         <v>2</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>2</v>
-      </c>
-      <c r="N14">
-        <v>4</v>
-      </c>
-      <c r="O14">
-        <v>2</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1990</v>
+        <v>1992</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E15">
         <v>2000000</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15">
         <v>6</v>
       </c>
-      <c r="H15">
+      <c r="M15">
         <v>10</v>
       </c>
-      <c r="I15">
-        <v>8</v>
-      </c>
-      <c r="J15">
-        <v>22</v>
-      </c>
-      <c r="K15">
+      <c r="N15">
         <v>4</v>
       </c>
-      <c r="L15">
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
         <v>4</v>
-      </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15">
-        <v>7</v>
-      </c>
-      <c r="P15">
-        <v>2</v>
       </c>
       <c r="Q15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1991</v>
+        <v>1993</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E16">
-        <v>6000000</v>
+        <v>2000000</v>
       </c>
       <c r="F16">
-        <v>46</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>8</v>
-      </c>
-      <c r="K16">
-        <v>8</v>
-      </c>
-      <c r="L16">
-        <v>6</v>
-      </c>
-      <c r="M16">
-        <v>5</v>
-      </c>
-      <c r="N16">
-        <v>5</v>
-      </c>
-      <c r="O16">
-        <v>8</v>
-      </c>
-      <c r="P16">
-        <v>3</v>
-      </c>
-      <c r="Q16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="R16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E17">
         <v>2000000</v>
       </c>
       <c r="F17">
-        <v>35</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>16</v>
-      </c>
-      <c r="K17">
-        <v>5</v>
-      </c>
-      <c r="L17">
-        <v>6</v>
-      </c>
-      <c r="M17">
-        <v>10</v>
-      </c>
-      <c r="N17">
-        <v>4</v>
-      </c>
-      <c r="O17">
-        <v>10</v>
-      </c>
-      <c r="P17">
-        <v>4</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1993</v>
       </c>
       <c r="B18" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>87</v>
+      <c r="C18" t="s">
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18">
         <v>2000000</v>
       </c>
       <c r="F18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="R18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>89</v>
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E19">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>34</v>
+      </c>
+      <c r="K19">
+        <v>9</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>7</v>
+      </c>
+      <c r="N19">
+        <v>16</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <v>4</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" t="s">
-        <v>92</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20">
-        <v>2000000</v>
+        <v>93</v>
       </c>
       <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>47</v>
+      </c>
+      <c r="H20">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>48</v>
+      </c>
+      <c r="K20">
+        <v>51</v>
+      </c>
+      <c r="L20">
+        <v>35</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" t="s">
+        <v>15</v>
+      </c>
+      <c r="P20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q20">
+        <v>36</v>
+      </c>
+      <c r="R20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>93</v>
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E21">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I21">
+        <v>28</v>
+      </c>
+      <c r="J21">
+        <v>35</v>
+      </c>
+      <c r="K21">
+        <v>24</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21">
+        <v>11</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+      <c r="Q21">
         <v>4</v>
       </c>
-      <c r="J21">
-        <v>34</v>
-      </c>
-      <c r="K21">
-        <v>9</v>
-      </c>
-      <c r="L21">
-        <v>4</v>
-      </c>
-      <c r="M21">
-        <v>7</v>
-      </c>
-      <c r="N21">
-        <v>16</v>
-      </c>
-      <c r="O21">
-        <v>7</v>
-      </c>
-      <c r="P21">
-        <v>4</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>1994</v>
+        <v>1996</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>96</v>
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="H22">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="I22">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J22">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K22">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="L22">
-        <v>35</v>
-      </c>
-      <c r="M22" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>15</v>
       </c>
       <c r="N22" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="O22">
+        <v>32</v>
       </c>
       <c r="P22">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="Q22">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="R22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E23">
-        <v>500000</v>
+        <v>600000</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
         <v>13</v>
       </c>
-      <c r="I23">
-        <v>28</v>
-      </c>
       <c r="J23">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="K23">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L23">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="M23">
-        <v>12</v>
-      </c>
-      <c r="N23" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="N23">
+        <v>22</v>
       </c>
       <c r="O23">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="P23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="R23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>1996</v>
+        <v>1998</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>26</v>
-      </c>
-      <c r="H24">
-        <v>54</v>
-      </c>
-      <c r="I24">
-        <v>17</v>
-      </c>
-      <c r="J24">
-        <v>43</v>
-      </c>
-      <c r="K24">
-        <v>42</v>
-      </c>
-      <c r="L24">
-        <v>8</v>
-      </c>
-      <c r="M24">
+        <v>62</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" t="s">
         <v>15</v>
       </c>
       <c r="N24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O24">
-        <v>32</v>
-      </c>
-      <c r="P24">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="O24" t="s">
+        <v>15</v>
+      </c>
+      <c r="P24" t="s">
+        <v>15</v>
       </c>
       <c r="Q24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="R24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>1996</v>
+        <v>1998</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25">
-        <v>600000</v>
+        <v>105</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>11</v>
-      </c>
-      <c r="H25">
-        <v>8</v>
-      </c>
-      <c r="I25">
-        <v>13</v>
-      </c>
-      <c r="J25">
-        <v>24</v>
-      </c>
-      <c r="K25">
+      <c r="R25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1999</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>85</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26">
+        <v>40</v>
+      </c>
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26">
+        <v>44</v>
+      </c>
+      <c r="L26">
+        <v>15</v>
+      </c>
+      <c r="M26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" t="s">
+        <v>15</v>
+      </c>
+      <c r="P26">
         <v>21</v>
       </c>
-      <c r="L25">
-        <v>13</v>
-      </c>
-      <c r="M25">
-        <v>27</v>
-      </c>
-      <c r="N25">
-        <v>22</v>
-      </c>
-      <c r="O25">
-        <v>22</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>1998</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>62</v>
-      </c>
-      <c r="H26" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" t="s">
-        <v>16</v>
-      </c>
-      <c r="P26" t="s">
-        <v>16</v>
-      </c>
       <c r="Q26">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="R26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="E27">
+        <v>500000</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>18</v>
+      </c>
+      <c r="H27">
+        <v>82</v>
+      </c>
+      <c r="I27">
+        <v>44</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>53</v>
+      </c>
+      <c r="L27">
+        <v>17</v>
+      </c>
+      <c r="M27">
+        <v>37</v>
+      </c>
+      <c r="N27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27">
+        <v>49</v>
+      </c>
+      <c r="P27">
+        <v>19</v>
+      </c>
+      <c r="Q27">
+        <v>145</v>
+      </c>
+      <c r="R27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F28">
-        <v>5</v>
-      </c>
-      <c r="G28">
-        <v>85</v>
-      </c>
-      <c r="H28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28">
-        <v>40</v>
-      </c>
-      <c r="J28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28">
-        <v>44</v>
-      </c>
-      <c r="L28">
-        <v>15</v>
-      </c>
-      <c r="M28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28">
-        <v>21</v>
-      </c>
-      <c r="Q28">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E29">
-        <v>500000</v>
+        <v>4000000</v>
       </c>
       <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>18</v>
-      </c>
-      <c r="H29">
-        <v>82</v>
-      </c>
-      <c r="I29">
-        <v>44</v>
-      </c>
-      <c r="J29">
-        <v>5</v>
-      </c>
-      <c r="K29">
-        <v>53</v>
-      </c>
-      <c r="L29">
-        <v>17</v>
-      </c>
-      <c r="M29">
-        <v>37</v>
-      </c>
-      <c r="N29" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29">
-        <v>49</v>
-      </c>
-      <c r="P29">
-        <v>19</v>
-      </c>
-      <c r="Q29">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="R29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2001</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>113</v>
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>117</v>
       </c>
       <c r="D30" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>109</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" t="s">
+        <v>15</v>
+      </c>
+      <c r="P30">
+        <v>74</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2002</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>2001</v>
-      </c>
-      <c r="B31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31">
-        <v>4000000</v>
-      </c>
-      <c r="F31">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" t="s">
+        <v>15</v>
+      </c>
+      <c r="M31" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" t="s">
+        <v>15</v>
+      </c>
+      <c r="P31" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F32">
-        <v>2</v>
-      </c>
-      <c r="G32">
-        <v>109</v>
-      </c>
-      <c r="H32" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" t="s">
-        <v>16</v>
-      </c>
-      <c r="M32" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" t="s">
-        <v>16</v>
-      </c>
-      <c r="P32">
-        <v>74</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2002</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>121</v>
+        <v>237</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
-      <c r="G33" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" t="s">
-        <v>16</v>
-      </c>
-      <c r="K33" t="s">
-        <v>16</v>
-      </c>
-      <c r="L33" t="s">
-        <v>16</v>
-      </c>
-      <c r="M33" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33" t="s">
-        <v>16</v>
-      </c>
-      <c r="O33" t="s">
-        <v>16</v>
-      </c>
-      <c r="P33" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" t="s">
-        <v>124</v>
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" t="s">
+        <v>15</v>
+      </c>
+      <c r="O34" t="s">
+        <v>15</v>
+      </c>
+      <c r="P34" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>15</v>
+      </c>
+      <c r="R34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" t="s">
         <v>127</v>
-      </c>
-      <c r="D35" t="s">
-        <v>125</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35">
+        <v>93</v>
+      </c>
+      <c r="L35">
+        <v>83</v>
+      </c>
+      <c r="M35" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" t="s">
+        <v>15</v>
+      </c>
+      <c r="O35" t="s">
+        <v>15</v>
+      </c>
+      <c r="P35" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>15</v>
+      </c>
+      <c r="R35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
         <v>129</v>
       </c>
-      <c r="D36" t="s">
-        <v>128</v>
+      <c r="E36">
+        <v>3000000</v>
       </c>
       <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" t="s">
-        <v>16</v>
-      </c>
-      <c r="K36" t="s">
-        <v>16</v>
-      </c>
-      <c r="L36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M36" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" t="s">
-        <v>16</v>
-      </c>
-      <c r="P36" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>19</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <v>11</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <v>3</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <v>25</v>
+      </c>
+      <c r="O36">
+        <v>6</v>
+      </c>
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" t="s">
         <v>131</v>
-      </c>
-      <c r="D37" t="s">
-        <v>130</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37">
-        <v>93</v>
-      </c>
-      <c r="L37">
-        <v>83</v>
+        <v>15</v>
+      </c>
+      <c r="K37" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" t="s">
+        <v>15</v>
       </c>
       <c r="M37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="R37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2004</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" t="s">
         <v>133</v>
       </c>
-      <c r="D38" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38">
-        <v>3000000</v>
-      </c>
       <c r="F38">
-        <v>26</v>
-      </c>
-      <c r="G38">
-        <v>3</v>
-      </c>
-      <c r="H38">
-        <v>19</v>
-      </c>
-      <c r="I38">
-        <v>4</v>
-      </c>
-      <c r="J38">
-        <v>11</v>
-      </c>
-      <c r="K38">
-        <v>4</v>
-      </c>
-      <c r="L38">
-        <v>3</v>
-      </c>
-      <c r="M38">
-        <v>2</v>
-      </c>
-      <c r="N38">
-        <v>25</v>
-      </c>
-      <c r="O38">
-        <v>6</v>
-      </c>
-      <c r="P38">
-        <v>2</v>
-      </c>
-      <c r="Q38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" t="s">
+        <v>15</v>
+      </c>
+      <c r="O38" t="s">
+        <v>15</v>
+      </c>
+      <c r="P38" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>15</v>
+      </c>
+      <c r="R38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2004</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
         <v>135</v>
       </c>
+      <c r="C39" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
-      <c r="G39" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" t="s">
-        <v>16</v>
-      </c>
-      <c r="L39" t="s">
-        <v>16</v>
-      </c>
-      <c r="M39" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" t="s">
-        <v>16</v>
-      </c>
-      <c r="O39" t="s">
-        <v>16</v>
-      </c>
-      <c r="P39" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>2004</v>
-      </c>
-      <c r="B40" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B40">
+        <v>3121</v>
+      </c>
+      <c r="C40" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40">
+        <v>500000</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>18</v>
+      </c>
+      <c r="I40">
+        <v>15</v>
+      </c>
+      <c r="J40">
+        <v>9</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <v>3</v>
+      </c>
+      <c r="M40">
+        <v>5</v>
+      </c>
+      <c r="N40" t="s">
+        <v>15</v>
+      </c>
+      <c r="O40">
+        <v>18</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>9</v>
+      </c>
+      <c r="R40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2006</v>
+      </c>
+      <c r="B41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41">
+        <v>12</v>
+      </c>
+      <c r="R41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2007</v>
+      </c>
+      <c r="B42" t="s">
         <v>37</v>
       </c>
-      <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" t="s">
-        <v>16</v>
-      </c>
-      <c r="K40" t="s">
-        <v>16</v>
-      </c>
-      <c r="L40" t="s">
-        <v>16</v>
-      </c>
-      <c r="M40" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" t="s">
-        <v>16</v>
-      </c>
-      <c r="O40" t="s">
-        <v>16</v>
-      </c>
-      <c r="P40" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>2004</v>
-      </c>
-      <c r="B41" t="s">
-        <v>138</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>2006</v>
-      </c>
-      <c r="B42">
-        <v>3121</v>
-      </c>
-      <c r="C42" t="s">
-        <v>142</v>
+      <c r="C42" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
-      </c>
-      <c r="E42">
-        <v>500000</v>
+        <v>143</v>
       </c>
       <c r="F42">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H42">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I42">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J42">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L42">
         <v>3</v>
       </c>
       <c r="M42">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O42">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="P42">
         <v>1</v>
       </c>
-      <c r="Q42">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q42" t="s">
+        <v>15</v>
+      </c>
+      <c r="R42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43" t="s">
         <v>145</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F43">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="R43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
+      </c>
+      <c r="C44" t="s">
+        <v>149</v>
       </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F44">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G44">
-        <v>3</v>
-      </c>
-      <c r="H44">
-        <v>38</v>
-      </c>
-      <c r="I44">
-        <v>11</v>
-      </c>
-      <c r="J44">
-        <v>17</v>
-      </c>
-      <c r="K44">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" t="s">
+        <v>15</v>
       </c>
       <c r="L44">
-        <v>3</v>
-      </c>
-      <c r="M44">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="M44" t="s">
+        <v>15</v>
       </c>
       <c r="N44" t="s">
-        <v>16</v>
-      </c>
-      <c r="O44">
-        <v>35</v>
-      </c>
-      <c r="P44">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="O44" t="s">
+        <v>15</v>
+      </c>
+      <c r="P44" t="s">
+        <v>15</v>
       </c>
       <c r="Q44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="R44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B45" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" t="s">
-        <v>152</v>
+        <v>38</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F46">
-        <v>25</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
       </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K46" t="s">
-        <v>16</v>
-      </c>
-      <c r="L46">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="L46" t="s">
+        <v>15</v>
       </c>
       <c r="M46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="R46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="B47" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
         <v>155</v>
       </c>
       <c r="F47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>33</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+      <c r="J47" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47">
+        <v>31</v>
+      </c>
+      <c r="L47">
+        <v>9</v>
+      </c>
+      <c r="M47">
+        <v>8</v>
+      </c>
+      <c r="N47">
+        <v>31</v>
+      </c>
+      <c r="O47">
+        <v>50</v>
+      </c>
+      <c r="P47">
+        <v>8</v>
+      </c>
+      <c r="Q47">
+        <v>11</v>
+      </c>
+      <c r="R47" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="B48" t="s">
         <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" t="s">
         <v>157</v>
       </c>
-      <c r="D48" t="s">
-        <v>156</v>
-      </c>
       <c r="F48">
+        <v>10</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48">
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <v>21</v>
+      </c>
+      <c r="K48">
+        <v>18</v>
+      </c>
+      <c r="L48">
+        <v>4</v>
+      </c>
+      <c r="M48">
+        <v>2</v>
+      </c>
+      <c r="N48">
+        <v>17</v>
+      </c>
+      <c r="O48">
+        <v>9</v>
+      </c>
+      <c r="P48">
+        <v>4</v>
+      </c>
+      <c r="Q48">
+        <v>8</v>
+      </c>
+      <c r="R48" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2015</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" t="s">
+        <v>159</v>
+      </c>
+      <c r="F49">
+        <v>7</v>
+      </c>
+      <c r="G49">
+        <v>48</v>
+      </c>
+      <c r="H49">
+        <v>25</v>
+      </c>
+      <c r="I49">
+        <v>53</v>
+      </c>
+      <c r="J49" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49">
+        <v>53</v>
+      </c>
+      <c r="L49">
+        <v>11</v>
+      </c>
+      <c r="M49" t="s">
+        <v>15</v>
+      </c>
+      <c r="N49" t="s">
+        <v>15</v>
+      </c>
+      <c r="O49" t="s">
+        <v>15</v>
+      </c>
+      <c r="P49">
+        <v>27</v>
+      </c>
+      <c r="Q49">
+        <v>50</v>
+      </c>
+      <c r="R49" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2015</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>40</v>
+      </c>
+      <c r="H50">
+        <v>117</v>
+      </c>
+      <c r="I50">
+        <v>20</v>
+      </c>
+      <c r="J50">
+        <v>47</v>
+      </c>
+      <c r="K50">
+        <v>21</v>
+      </c>
+      <c r="L50">
+        <v>38</v>
+      </c>
+      <c r="M50" t="s">
+        <v>15</v>
+      </c>
+      <c r="N50" t="s">
+        <v>15</v>
+      </c>
+      <c r="O50">
+        <v>50</v>
+      </c>
+      <c r="P50">
+        <v>9</v>
+      </c>
+      <c r="Q50">
+        <v>21</v>
+      </c>
+      <c r="R50" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2016</v>
+      </c>
+      <c r="B51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51">
+        <v>26</v>
+      </c>
+      <c r="R51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2017</v>
+      </c>
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52">
         <v>0</v>
       </c>
-      <c r="G48" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" t="s">
-        <v>16</v>
-      </c>
-      <c r="K48" t="s">
-        <v>16</v>
-      </c>
-      <c r="L48" t="s">
-        <v>16</v>
-      </c>
-      <c r="M48" t="s">
-        <v>16</v>
-      </c>
-      <c r="N48" t="s">
-        <v>16</v>
-      </c>
-      <c r="O48" t="s">
-        <v>16</v>
-      </c>
-      <c r="P48" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>2014</v>
-      </c>
-      <c r="B49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D49" t="s">
-        <v>158</v>
-      </c>
-      <c r="F49">
-        <v>4</v>
-      </c>
-      <c r="G49">
-        <v>8</v>
-      </c>
-      <c r="H49">
-        <v>33</v>
-      </c>
-      <c r="I49">
-        <v>10</v>
-      </c>
-      <c r="J49" t="s">
-        <v>16</v>
-      </c>
-      <c r="K49">
-        <v>31</v>
-      </c>
-      <c r="L49">
-        <v>9</v>
-      </c>
-      <c r="M49">
-        <v>8</v>
-      </c>
-      <c r="N49">
-        <v>31</v>
-      </c>
-      <c r="O49">
-        <v>50</v>
-      </c>
-      <c r="P49">
-        <v>8</v>
-      </c>
-      <c r="Q49">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>2014</v>
-      </c>
-      <c r="B50" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D50" t="s">
-        <v>160</v>
-      </c>
-      <c r="F50">
-        <v>10</v>
-      </c>
-      <c r="G50">
-        <v>5</v>
-      </c>
-      <c r="H50">
-        <v>15</v>
-      </c>
-      <c r="I50">
-        <v>8</v>
-      </c>
-      <c r="J50">
-        <v>21</v>
-      </c>
-      <c r="K50">
-        <v>18</v>
-      </c>
-      <c r="L50">
-        <v>4</v>
-      </c>
-      <c r="M50">
+      <c r="R52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2018</v>
+      </c>
+      <c r="B53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" t="s">
+        <v>170</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="R53" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2018</v>
+      </c>
+      <c r="B54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" t="s">
+        <v>174</v>
+      </c>
+      <c r="F54">
         <v>2</v>
       </c>
-      <c r="N50">
-        <v>17</v>
-      </c>
-      <c r="O50">
-        <v>9</v>
-      </c>
-      <c r="P50">
-        <v>4</v>
-      </c>
-      <c r="Q50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>2015</v>
-      </c>
-      <c r="B51" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" t="s">
-        <v>162</v>
-      </c>
-      <c r="F51">
-        <v>7</v>
-      </c>
-      <c r="G51">
-        <v>48</v>
-      </c>
-      <c r="H51">
-        <v>25</v>
-      </c>
-      <c r="I51">
-        <v>53</v>
-      </c>
-      <c r="J51" t="s">
-        <v>16</v>
-      </c>
-      <c r="K51">
-        <v>53</v>
-      </c>
-      <c r="L51">
-        <v>11</v>
-      </c>
-      <c r="M51" t="s">
-        <v>16</v>
-      </c>
-      <c r="N51" t="s">
-        <v>16</v>
-      </c>
-      <c r="O51" t="s">
-        <v>16</v>
-      </c>
-      <c r="P51">
-        <v>27</v>
-      </c>
-      <c r="Q51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>2015</v>
-      </c>
-      <c r="B52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D52" t="s">
-        <v>164</v>
-      </c>
-      <c r="F52">
-        <v>3</v>
-      </c>
-      <c r="G52">
-        <v>40</v>
-      </c>
-      <c r="H52">
-        <v>117</v>
-      </c>
-      <c r="I52">
-        <v>20</v>
-      </c>
-      <c r="J52">
-        <v>47</v>
-      </c>
-      <c r="K52">
-        <v>21</v>
-      </c>
-      <c r="L52">
-        <v>38</v>
-      </c>
-      <c r="M52" t="s">
-        <v>16</v>
-      </c>
-      <c r="N52" t="s">
-        <v>16</v>
-      </c>
-      <c r="O52">
-        <v>50</v>
-      </c>
-      <c r="P52">
-        <v>9</v>
-      </c>
-      <c r="Q52">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>2016</v>
-      </c>
-      <c r="B53" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D53" t="s">
-        <v>168</v>
-      </c>
-      <c r="F53">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>2017</v>
-      </c>
-      <c r="B54" t="s">
-        <v>169</v>
-      </c>
-      <c r="C54" t="s">
-        <v>171</v>
-      </c>
-      <c r="D54" t="s">
-        <v>170</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>2018</v>
-      </c>
-      <c r="B55" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>2018</v>
-      </c>
-      <c r="B56" t="s">
-        <v>175</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" t="s">
-        <v>177</v>
-      </c>
-      <c r="F56">
-        <v>2</v>
+      <c r="R54" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D48" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D29" r:id="rId1"/>
+    <hyperlink ref="D46" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="R2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6351,7 +6677,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -6359,18 +6685,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -6379,7 +6705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6394,13 +6720,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>